<commit_message>
Adding Category Related Classes(Needs to be complete)
</commit_message>
<xml_diff>
--- a/بارم بندی فازهای پروژه.xlsx
+++ b/بارم بندی فازهای پروژه.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amirreza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amirreza\Documents\Education\University\2nd Semester\Advanced Programming\Project\ProjectTeam30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4286A80E-A6BE-4ABE-B68A-0E16BF721714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788AB5D3-1C18-41A5-A3DC-75C8DA7D9B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="فاز صفر" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="246">
   <si>
     <t>Trello</t>
   </si>
@@ -765,6 +765,9 @@
   </si>
   <si>
     <t>پیاده سازی صدا با فشردن دکمه ها و هرگونه صداگذاری: - دکمه(10) - بک گراند(15) - صدای متفاوت در صفحات مختلف(15)</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -1002,9 +1005,6 @@
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
@@ -1041,22 +1041,13 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
@@ -1064,14 +1055,34 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1316,227 +1327,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="24" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="25" t="s">
+      <c r="H2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="25" t="s">
+      <c r="X2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Y2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="25" t="s">
+      <c r="Z2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AA2" s="25" t="s">
+      <c r="AA2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="25" t="s">
+      <c r="AB2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="25" t="s">
+      <c r="AC2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="26"/>
+      <c r="AD2" s="19"/>
     </row>
     <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="27">
-        <v>5</v>
-      </c>
-      <c r="C3" s="27">
+      <c r="B3" s="14">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14">
         <v>15</v>
       </c>
-      <c r="D3" s="27">
-        <v>5</v>
-      </c>
-      <c r="E3" s="27">
-        <v>10</v>
-      </c>
-      <c r="F3" s="27">
-        <v>10</v>
-      </c>
-      <c r="G3" s="27">
-        <v>10</v>
-      </c>
-      <c r="H3" s="27">
-        <v>10</v>
-      </c>
-      <c r="I3" s="27">
-        <v>10</v>
-      </c>
-      <c r="J3" s="27">
-        <v>10</v>
-      </c>
-      <c r="K3" s="27">
-        <v>10</v>
-      </c>
-      <c r="L3" s="27">
-        <v>10</v>
-      </c>
-      <c r="M3" s="27">
-        <v>10</v>
-      </c>
-      <c r="N3" s="27">
-        <v>10</v>
-      </c>
-      <c r="O3" s="27">
-        <v>5</v>
-      </c>
-      <c r="P3" s="27">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="27">
-        <v>5</v>
-      </c>
-      <c r="R3" s="27">
-        <v>5</v>
-      </c>
-      <c r="S3" s="27">
-        <v>5</v>
-      </c>
-      <c r="T3" s="27">
-        <v>5</v>
-      </c>
-      <c r="U3" s="27">
-        <v>5</v>
-      </c>
-      <c r="V3" s="27">
-        <v>5</v>
-      </c>
-      <c r="W3" s="27">
-        <v>5</v>
-      </c>
-      <c r="X3" s="27">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="27">
-        <v>5</v>
-      </c>
-      <c r="Z3" s="27">
-        <v>5</v>
-      </c>
-      <c r="AA3" s="27">
-        <v>5</v>
-      </c>
-      <c r="AB3" s="27">
-        <v>5</v>
-      </c>
-      <c r="AC3" s="27">
-        <v>5</v>
-      </c>
-      <c r="AD3" s="27">
+      <c r="D3" s="14">
+        <v>5</v>
+      </c>
+      <c r="E3" s="14">
+        <v>10</v>
+      </c>
+      <c r="F3" s="14">
+        <v>10</v>
+      </c>
+      <c r="G3" s="14">
+        <v>10</v>
+      </c>
+      <c r="H3" s="14">
+        <v>10</v>
+      </c>
+      <c r="I3" s="14">
+        <v>10</v>
+      </c>
+      <c r="J3" s="14">
+        <v>10</v>
+      </c>
+      <c r="K3" s="14">
+        <v>10</v>
+      </c>
+      <c r="L3" s="14">
+        <v>10</v>
+      </c>
+      <c r="M3" s="14">
+        <v>10</v>
+      </c>
+      <c r="N3" s="14">
+        <v>10</v>
+      </c>
+      <c r="O3" s="14">
+        <v>5</v>
+      </c>
+      <c r="P3" s="14">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>5</v>
+      </c>
+      <c r="R3" s="14">
+        <v>5</v>
+      </c>
+      <c r="S3" s="14">
+        <v>5</v>
+      </c>
+      <c r="T3" s="14">
+        <v>5</v>
+      </c>
+      <c r="U3" s="14">
+        <v>5</v>
+      </c>
+      <c r="V3" s="14">
+        <v>5</v>
+      </c>
+      <c r="W3" s="14">
+        <v>5</v>
+      </c>
+      <c r="X3" s="14">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="14">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="14">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="14">
+        <v>5</v>
+      </c>
+      <c r="AB3" s="14">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="14">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="14">
         <f>SUM(B3:AC3)</f>
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1555,10 +1566,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CN3"/>
+  <dimension ref="A1:CN4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1621,712 +1632,863 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="14" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="14" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="14" t="s">
+      <c r="J1" s="25"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="2" t="s">
+      <c r="M1" s="25"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="14" t="s">
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="16"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="14" t="s">
+      <c r="U1" s="25"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="14" t="s">
+      <c r="X1" s="25"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="14" t="s">
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="14" t="s">
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="14" t="s">
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="14" t="s">
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="14" t="s">
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="14" t="s">
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="14" t="s">
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="14" t="s">
+      <c r="BB1" s="24"/>
+      <c r="BC1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BD1" s="16"/>
-      <c r="BE1" s="16"/>
-      <c r="BF1" s="16"/>
-      <c r="BG1" s="16"/>
-      <c r="BH1" s="16"/>
-      <c r="BI1" s="15"/>
-      <c r="BJ1" s="14" t="s">
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="24"/>
+      <c r="BJ1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="BK1" s="15"/>
-      <c r="BL1" s="14" t="s">
+      <c r="BK1" s="24"/>
+      <c r="BL1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="BM1" s="16"/>
-      <c r="BN1" s="16"/>
-      <c r="BO1" s="16"/>
-      <c r="BP1" s="16"/>
-      <c r="BQ1" s="16"/>
-      <c r="BR1" s="16"/>
-      <c r="BS1" s="16"/>
-      <c r="BT1" s="16"/>
-      <c r="BU1" s="16"/>
-      <c r="BV1" s="15"/>
-      <c r="BW1" s="14" t="s">
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="24"/>
+      <c r="BW1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="BX1" s="16"/>
-      <c r="BY1" s="16"/>
-      <c r="BZ1" s="15"/>
-      <c r="CA1" s="3" t="s">
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="24"/>
+      <c r="CA1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CB1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CC1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CD1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CE1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="CF1" s="14" t="s">
+      <c r="CF1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="CG1" s="16"/>
-      <c r="CH1" s="16"/>
-      <c r="CI1" s="16"/>
-      <c r="CJ1" s="16"/>
-      <c r="CK1" s="15"/>
-      <c r="CL1" s="18" t="s">
+      <c r="CG1" s="25"/>
+      <c r="CH1" s="25"/>
+      <c r="CI1" s="25"/>
+      <c r="CJ1" s="25"/>
+      <c r="CK1" s="24"/>
+      <c r="CL1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="CM1" s="18" t="s">
+      <c r="CM1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="CN1" s="18" t="s">
+      <c r="CN1" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AH2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AI2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AL2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AM2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AN2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AO2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AP2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AS2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AT2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AU2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AV2" s="5" t="s">
+      <c r="AV2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AW2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AX2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AY2" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BA2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BB2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BC2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BD2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BE2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BF2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BG2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="BH2" s="4" t="s">
+      <c r="BH2" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BI2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BJ2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BK2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BL2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BM2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="BN2" s="4" t="s">
+      <c r="BN2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="BO2" s="4" t="s">
+      <c r="BO2" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="BP2" s="4" t="s">
+      <c r="BP2" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="BQ2" s="4" t="s">
+      <c r="BQ2" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="BR2" s="4" t="s">
+      <c r="BR2" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="BS2" s="4" t="s">
+      <c r="BS2" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="BT2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="BU2" s="4" t="s">
+      <c r="BU2" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BV2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BW2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="BX2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="BY2" s="4" t="s">
+      <c r="BY2" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="BZ2" s="4" t="s">
+      <c r="BZ2" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="CA2" s="4" t="s">
+      <c r="CA2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="CB2" s="4" t="s">
+      <c r="CB2" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="CC2" s="4" t="s">
+      <c r="CC2" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="CD2" s="4" t="s">
+      <c r="CD2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="CE2" s="4" t="s">
+      <c r="CE2" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="CF2" s="4" t="s">
+      <c r="CF2" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="CG2" s="4" t="s">
+      <c r="CG2" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="CH2" s="4" t="s">
+      <c r="CH2" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="CI2" s="4" t="s">
+      <c r="CI2" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="CJ2" s="4" t="s">
+      <c r="CJ2" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="CK2" s="4" t="s">
+      <c r="CK2" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="CL2" s="19"/>
-      <c r="CM2" s="19"/>
-      <c r="CN2" s="19"/>
+      <c r="CL2" s="28"/>
+      <c r="CM2" s="28"/>
+      <c r="CN2" s="28"/>
     </row>
     <row r="3" spans="1:92" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1">
-        <v>5</v>
-      </c>
-      <c r="I3" s="1">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1">
-        <v>5</v>
-      </c>
-      <c r="L3" s="1">
-        <v>10</v>
-      </c>
-      <c r="M3" s="1">
-        <v>10</v>
-      </c>
-      <c r="N3" s="1">
-        <v>5</v>
-      </c>
-      <c r="O3" s="1">
-        <v>10</v>
-      </c>
-      <c r="P3" s="1">
+      <c r="A3" s="5">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5">
+        <v>10</v>
+      </c>
+      <c r="J3" s="5">
+        <v>10</v>
+      </c>
+      <c r="K3" s="5">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5">
+        <v>10</v>
+      </c>
+      <c r="M3" s="5">
+        <v>10</v>
+      </c>
+      <c r="N3" s="5">
+        <v>5</v>
+      </c>
+      <c r="O3" s="5">
+        <v>10</v>
+      </c>
+      <c r="P3" s="5">
         <v>20</v>
       </c>
-      <c r="Q3" s="1">
-        <v>5</v>
-      </c>
-      <c r="R3" s="1">
-        <v>5</v>
-      </c>
-      <c r="S3" s="1">
-        <v>5</v>
-      </c>
-      <c r="T3" s="1">
+      <c r="Q3" s="5">
+        <v>5</v>
+      </c>
+      <c r="R3" s="5">
+        <v>5</v>
+      </c>
+      <c r="S3" s="5">
+        <v>5</v>
+      </c>
+      <c r="T3" s="5">
         <v>30</v>
       </c>
-      <c r="U3" s="1">
-        <v>10</v>
-      </c>
-      <c r="V3" s="1">
-        <v>10</v>
-      </c>
-      <c r="W3" s="1">
+      <c r="U3" s="5">
+        <v>10</v>
+      </c>
+      <c r="V3" s="5">
+        <v>10</v>
+      </c>
+      <c r="W3" s="5">
         <v>30</v>
       </c>
-      <c r="X3" s="1">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>10</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AA3" s="1">
+      <c r="X3" s="5">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="5">
         <v>20</v>
       </c>
-      <c r="AB3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AG3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AH3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AI3" s="1">
+      <c r="AB3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="5">
         <v>20</v>
       </c>
-      <c r="AJ3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AK3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AL3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AM3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AO3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AP3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AQ3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AT3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AU3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AV3" s="6">
-        <v>10</v>
-      </c>
-      <c r="AW3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AX3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AY3" s="1">
+      <c r="AJ3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AU3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AV3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AW3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AX3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AY3" s="5">
         <v>15</v>
       </c>
-      <c r="AZ3" s="1">
-        <v>10</v>
-      </c>
-      <c r="BA3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BB3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BC3" s="1">
-        <v>10</v>
-      </c>
-      <c r="BD3" s="1">
-        <v>10</v>
-      </c>
-      <c r="BE3" s="1">
+      <c r="AZ3" s="5">
+        <v>10</v>
+      </c>
+      <c r="BA3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC3" s="5">
+        <v>10</v>
+      </c>
+      <c r="BD3" s="5">
+        <v>10</v>
+      </c>
+      <c r="BE3" s="5">
         <v>15</v>
       </c>
-      <c r="BF3" s="1">
+      <c r="BF3" s="5">
         <v>30</v>
       </c>
-      <c r="BG3" s="1">
+      <c r="BG3" s="5">
         <v>15</v>
       </c>
-      <c r="BH3" s="1">
-        <v>10</v>
-      </c>
-      <c r="BI3" s="1">
+      <c r="BH3" s="5">
+        <v>10</v>
+      </c>
+      <c r="BI3" s="5">
         <v>20</v>
       </c>
-      <c r="BJ3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BK3" s="1" t="s">
+      <c r="BJ3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK3" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="BL3" s="1" t="s">
+      <c r="BL3" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="BM3" s="1">
+      <c r="BM3" s="5">
         <v>15</v>
       </c>
-      <c r="BN3" s="1">
+      <c r="BN3" s="5">
         <v>15</v>
       </c>
-      <c r="BO3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BP3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BQ3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BR3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BS3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BT3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BU3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BV3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BW3" s="1">
-        <v>10</v>
-      </c>
-      <c r="BX3" s="1">
+      <c r="BO3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BP3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BQ3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BR3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BS3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BT3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BU3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BV3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BW3" s="5">
+        <v>10</v>
+      </c>
+      <c r="BX3" s="5">
         <v>25</v>
       </c>
-      <c r="BY3" s="1">
-        <v>5</v>
-      </c>
-      <c r="BZ3" s="1">
-        <v>5</v>
-      </c>
-      <c r="CA3" s="1">
+      <c r="BY3" s="5">
+        <v>5</v>
+      </c>
+      <c r="BZ3" s="5">
+        <v>5</v>
+      </c>
+      <c r="CA3" s="5">
         <v>30</v>
       </c>
-      <c r="CB3" s="6">
+      <c r="CB3" s="5">
         <v>40</v>
       </c>
-      <c r="CC3" s="1">
+      <c r="CC3" s="5">
         <v>70</v>
       </c>
-      <c r="CD3" s="1">
+      <c r="CD3" s="5">
         <v>40</v>
       </c>
-      <c r="CE3" s="1">
+      <c r="CE3" s="5">
         <v>15</v>
       </c>
-      <c r="CF3" s="1">
+      <c r="CF3" s="5">
         <v>145</v>
       </c>
-      <c r="CG3" s="1">
+      <c r="CG3" s="5">
         <v>35</v>
       </c>
-      <c r="CH3" s="1">
+      <c r="CH3" s="5">
         <v>40</v>
       </c>
-      <c r="CI3" s="1">
+      <c r="CI3" s="5">
         <v>20</v>
       </c>
-      <c r="CJ3" s="1">
+      <c r="CJ3" s="5">
         <v>30</v>
       </c>
-      <c r="CK3" s="1">
+      <c r="CK3" s="5">
         <v>30</v>
       </c>
-      <c r="CL3" s="1">
+      <c r="CL3" s="5">
         <f>SUM(A3:CE3)</f>
         <v>900</v>
       </c>
-      <c r="CM3" s="1">
+      <c r="CM3" s="5">
         <f>SUM(CF3:CK3)</f>
         <v>300</v>
       </c>
-      <c r="CN3" s="1">
+      <c r="CN3" s="5">
         <f>CL3 + CM3</f>
         <v>1200</v>
       </c>
+    </row>
+    <row r="4" spans="1:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="T4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="U4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="V4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="27"/>
+      <c r="AF4" s="27"/>
+      <c r="AG4" s="27"/>
+      <c r="AH4" s="27"/>
+      <c r="AI4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AJ4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AK4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AL4" s="27"/>
+      <c r="AM4" s="27"/>
+      <c r="AN4" s="27"/>
+      <c r="AO4" s="27"/>
+      <c r="AP4" s="27"/>
+      <c r="AQ4" s="27"/>
+      <c r="AR4" s="27"/>
+      <c r="AS4" s="27"/>
+      <c r="AT4" s="27"/>
+      <c r="AU4" s="27"/>
+      <c r="AV4" s="27"/>
+      <c r="AW4" s="27"/>
+      <c r="AX4" s="27"/>
+      <c r="AY4" s="27"/>
+      <c r="AZ4" s="27"/>
+      <c r="BA4" s="27"/>
+      <c r="BB4" s="27"/>
+      <c r="BC4" s="27"/>
+      <c r="BD4" s="27"/>
+      <c r="BE4" s="27"/>
+      <c r="BF4" s="27"/>
+      <c r="BG4" s="27"/>
+      <c r="BH4" s="27"/>
+      <c r="BI4" s="27"/>
+      <c r="BJ4" s="27"/>
+      <c r="BK4" s="27"/>
+      <c r="BL4" s="27"/>
+      <c r="BM4" s="27"/>
+      <c r="BN4" s="27"/>
+      <c r="BO4" s="27"/>
+      <c r="BP4" s="27"/>
+      <c r="BQ4" s="27"/>
+      <c r="BR4" s="27"/>
+      <c r="BS4" s="27"/>
+      <c r="BT4" s="27"/>
+      <c r="BU4" s="27"/>
+      <c r="BV4" s="27"/>
+      <c r="BW4" s="27"/>
+      <c r="BX4" s="27"/>
+      <c r="BY4" s="27"/>
+      <c r="BZ4" s="27"/>
+      <c r="CA4" s="27"/>
+      <c r="CB4" s="27"/>
+      <c r="CC4" s="27"/>
+      <c r="CD4" s="27"/>
+      <c r="CE4" s="27"/>
+      <c r="CF4" s="27"/>
+      <c r="CG4" s="27"/>
+      <c r="CH4" s="27"/>
+      <c r="CI4" s="27"/>
+      <c r="CJ4" s="27"/>
+      <c r="CK4" s="27"/>
+      <c r="CL4" s="27"/>
+      <c r="CM4" s="27"/>
+      <c r="CN4" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AN1:AS1"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:AZ1"/>
+    <mergeCell ref="CM1:CM2"/>
     <mergeCell ref="CN1:CN2"/>
     <mergeCell ref="BA1:BB1"/>
     <mergeCell ref="BC1:BI1"/>
@@ -2335,21 +2497,6 @@
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CF1:CK1"/>
     <mergeCell ref="CL1:CL2"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="AN1:AS1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:AZ1"/>
-    <mergeCell ref="CM1:CM2"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AH1"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="P1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2360,10 +2507,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CK3"/>
+  <dimension ref="A1:CK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2441,659 +2588,784 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:89" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="20" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="20" t="s">
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="20" t="s">
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="20" t="s">
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="20" t="s">
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="16"/>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="16"/>
-      <c r="BA1" s="16"/>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="16"/>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="20" t="s">
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="25"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="24"/>
+      <c r="BE1" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="BF1" s="16"/>
-      <c r="BG1" s="16"/>
-      <c r="BH1" s="16"/>
-      <c r="BI1" s="16"/>
-      <c r="BJ1" s="16"/>
-      <c r="BK1" s="15"/>
-      <c r="BL1" s="20" t="s">
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="24"/>
+      <c r="BL1" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="BM1" s="16"/>
-      <c r="BN1" s="16"/>
-      <c r="BO1" s="16"/>
-      <c r="BP1" s="16"/>
-      <c r="BQ1" s="15"/>
-      <c r="BR1" s="20" t="s">
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="24"/>
+      <c r="BR1" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="BS1" s="16"/>
-      <c r="BT1" s="16"/>
-      <c r="BU1" s="16"/>
-      <c r="BV1" s="16"/>
-      <c r="BW1" s="16"/>
-      <c r="BX1" s="15"/>
-      <c r="BY1" s="14" t="s">
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="24"/>
+      <c r="BY1" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="BZ1" s="16"/>
-      <c r="CA1" s="16"/>
-      <c r="CB1" s="16"/>
-      <c r="CC1" s="16"/>
-      <c r="CD1" s="16"/>
-      <c r="CE1" s="16"/>
-      <c r="CF1" s="16"/>
-      <c r="CG1" s="16"/>
-      <c r="CH1" s="16"/>
-      <c r="CI1" s="15"/>
-      <c r="CJ1" s="21" t="s">
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
+      <c r="CB1" s="25"/>
+      <c r="CC1" s="25"/>
+      <c r="CD1" s="25"/>
+      <c r="CE1" s="25"/>
+      <c r="CF1" s="25"/>
+      <c r="CG1" s="25"/>
+      <c r="CH1" s="25"/>
+      <c r="CI1" s="24"/>
+      <c r="CJ1" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="CK1" s="21" t="s">
+      <c r="CK1" s="22" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:89" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="X2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Y2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AA2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AB2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AC2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AE2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AF2" s="7" t="s">
+      <c r="AF2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AG2" s="7" t="s">
+      <c r="AG2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AH2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AI2" s="7" t="s">
+      <c r="AI2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AJ2" s="7" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="AK2" s="7" t="s">
+      <c r="AK2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AL2" s="7" t="s">
+      <c r="AL2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AM2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AN2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AO2" s="10" t="s">
+      <c r="AO2" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="AP2" s="10" t="s">
+      <c r="AP2" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="AS2" s="8" t="s">
+      <c r="AS2" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="AT2" s="8" t="s">
+      <c r="AT2" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AU2" s="7" t="s">
+      <c r="AU2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AV2" s="7" t="s">
+      <c r="AV2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AW2" s="7" t="s">
+      <c r="AW2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AX2" s="7" t="s">
+      <c r="AX2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AY2" s="7" t="s">
+      <c r="AY2" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="AZ2" s="8" t="s">
+      <c r="AZ2" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="BA2" s="8" t="s">
+      <c r="BA2" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="BB2" s="10" t="s">
+      <c r="BB2" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="BC2" s="10" t="s">
+      <c r="BC2" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="BD2" s="9" t="s">
+      <c r="BD2" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="BE2" s="9" t="s">
+      <c r="BE2" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="BF2" s="9" t="s">
+      <c r="BF2" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="BG2" s="9" t="s">
+      <c r="BG2" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="BH2" s="9" t="s">
+      <c r="BH2" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="BI2" s="9" t="s">
+      <c r="BI2" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="BJ2" s="9" t="s">
+      <c r="BJ2" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="BK2" s="9" t="s">
+      <c r="BK2" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="BL2" s="11" t="s">
+      <c r="BL2" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="BM2" s="11" t="s">
+      <c r="BM2" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="BN2" s="11" t="s">
+      <c r="BN2" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="BO2" s="11" t="s">
+      <c r="BO2" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="BP2" s="11" t="s">
+      <c r="BP2" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="BQ2" s="11" t="s">
+      <c r="BQ2" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="BR2" s="7" t="s">
+      <c r="BR2" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="BS2" s="7" t="s">
+      <c r="BS2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="BT2" s="7" t="s">
+      <c r="BT2" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="BU2" s="7" t="s">
+      <c r="BU2" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="BV2" s="7" t="s">
+      <c r="BV2" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="BW2" s="7" t="s">
+      <c r="BW2" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="BX2" s="7" t="s">
+      <c r="BX2" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="BY2" s="10" t="s">
+      <c r="BY2" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="BZ2" s="10" t="s">
+      <c r="BZ2" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="CA2" s="10" t="s">
+      <c r="CA2" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="CB2" s="10" t="s">
+      <c r="CB2" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="CC2" s="10" t="s">
+      <c r="CC2" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="CD2" s="8" t="s">
+      <c r="CD2" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="CE2" s="8" t="s">
+      <c r="CE2" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="CF2" s="8" t="s">
+      <c r="CF2" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="CG2" s="8" t="s">
+      <c r="CG2" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="CH2" s="8" t="s">
+      <c r="CH2" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="CI2" s="8" t="s">
+      <c r="CI2" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="CJ2" s="17"/>
-      <c r="CK2" s="17"/>
+      <c r="CJ2" s="26"/>
+      <c r="CK2" s="26"/>
     </row>
     <row r="3" spans="1:89" x14ac:dyDescent="0.35">
-      <c r="A3" s="12">
-        <v>10</v>
-      </c>
-      <c r="B3" s="12">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12">
-        <v>10</v>
-      </c>
-      <c r="D3" s="12">
+      <c r="A3" s="11">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11">
         <v>15</v>
       </c>
-      <c r="E3" s="12">
-        <v>5</v>
-      </c>
-      <c r="F3" s="12">
-        <v>5</v>
-      </c>
-      <c r="G3" s="12">
-        <v>5</v>
-      </c>
-      <c r="H3" s="12">
-        <v>5</v>
-      </c>
-      <c r="I3" s="12">
+      <c r="E3" s="11">
+        <v>5</v>
+      </c>
+      <c r="F3" s="11">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11">
+        <v>5</v>
+      </c>
+      <c r="H3" s="11">
+        <v>5</v>
+      </c>
+      <c r="I3" s="11">
         <v>20</v>
       </c>
-      <c r="J3" s="12">
-        <v>5</v>
-      </c>
-      <c r="K3" s="12">
-        <v>5</v>
-      </c>
-      <c r="L3" s="12">
-        <v>5</v>
-      </c>
-      <c r="M3" s="12">
-        <v>5</v>
-      </c>
-      <c r="N3" s="12">
-        <v>10</v>
-      </c>
-      <c r="O3" s="12">
-        <v>5</v>
-      </c>
-      <c r="P3" s="12">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="12">
-        <v>10</v>
-      </c>
-      <c r="R3" s="12">
-        <v>5</v>
-      </c>
-      <c r="S3" s="12">
-        <v>10</v>
-      </c>
-      <c r="T3" s="12">
-        <v>10</v>
-      </c>
-      <c r="U3" s="12">
-        <v>5</v>
-      </c>
-      <c r="V3" s="12">
-        <v>5</v>
-      </c>
-      <c r="W3" s="12">
-        <v>5</v>
-      </c>
-      <c r="X3" s="12">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="12">
-        <v>5</v>
-      </c>
-      <c r="Z3" s="12">
+      <c r="J3" s="11">
+        <v>5</v>
+      </c>
+      <c r="K3" s="11">
+        <v>5</v>
+      </c>
+      <c r="L3" s="11">
+        <v>5</v>
+      </c>
+      <c r="M3" s="11">
+        <v>5</v>
+      </c>
+      <c r="N3" s="11">
+        <v>10</v>
+      </c>
+      <c r="O3" s="11">
+        <v>5</v>
+      </c>
+      <c r="P3" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>10</v>
+      </c>
+      <c r="R3" s="11">
+        <v>5</v>
+      </c>
+      <c r="S3" s="11">
+        <v>10</v>
+      </c>
+      <c r="T3" s="11">
+        <v>10</v>
+      </c>
+      <c r="U3" s="11">
+        <v>5</v>
+      </c>
+      <c r="V3" s="11">
+        <v>5</v>
+      </c>
+      <c r="W3" s="11">
+        <v>5</v>
+      </c>
+      <c r="X3" s="11">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="11">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="11">
         <v>30</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AA3" s="11">
         <v>30</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AB3" s="11">
         <v>30</v>
       </c>
-      <c r="AC3" s="12">
-        <v>5</v>
-      </c>
-      <c r="AD3" s="12">
-        <v>5</v>
-      </c>
-      <c r="AE3" s="12">
+      <c r="AC3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AE3" s="11">
         <v>25</v>
       </c>
-      <c r="AF3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AG3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AH3" s="12">
-        <v>5</v>
-      </c>
-      <c r="AI3" s="12">
-        <v>5</v>
-      </c>
-      <c r="AJ3" s="12">
-        <v>5</v>
-      </c>
-      <c r="AK3" s="12">
-        <v>5</v>
-      </c>
-      <c r="AL3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AM3" s="12">
+      <c r="AF3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AG3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AH3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AJ3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AK3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AL3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AM3" s="11">
         <v>20</v>
       </c>
-      <c r="AN3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AO3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AP3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AQ3" s="12">
-        <v>5</v>
-      </c>
-      <c r="AR3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AS3" s="12">
+      <c r="AN3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AO3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AP3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AQ3" s="11">
+        <v>5</v>
+      </c>
+      <c r="AR3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AS3" s="11">
         <v>15</v>
       </c>
-      <c r="AT3" s="12">
+      <c r="AT3" s="11">
         <v>15</v>
       </c>
-      <c r="AU3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AV3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AW3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AX3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AY3" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ3" s="12">
+      <c r="AU3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AV3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AW3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AX3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AY3" s="11">
+        <v>10</v>
+      </c>
+      <c r="AZ3" s="11">
         <v>20</v>
       </c>
-      <c r="BA3" s="12">
+      <c r="BA3" s="11">
         <v>30</v>
       </c>
-      <c r="BB3" s="12">
+      <c r="BB3" s="11">
         <v>35</v>
       </c>
-      <c r="BC3" s="12">
+      <c r="BC3" s="11">
         <v>40</v>
       </c>
-      <c r="BD3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE3" s="12">
-        <v>10</v>
-      </c>
-      <c r="BF3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BG3" s="12">
-        <v>10</v>
-      </c>
-      <c r="BH3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BI3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BJ3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BK3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BL3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BM3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BN3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BO3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BP3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BQ3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BR3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BS3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BT3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BU3" s="12">
+      <c r="BD3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BE3" s="11">
+        <v>10</v>
+      </c>
+      <c r="BF3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BG3" s="11">
+        <v>10</v>
+      </c>
+      <c r="BH3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BI3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BJ3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BK3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BL3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BM3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BN3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BO3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BP3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BQ3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BR3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BS3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BT3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BU3" s="11">
         <v>20</v>
       </c>
-      <c r="BV3" s="12">
-        <v>5</v>
-      </c>
-      <c r="BW3" s="12">
-        <v>10</v>
-      </c>
-      <c r="BX3" s="12">
-        <v>10</v>
-      </c>
-      <c r="BY3" s="13">
+      <c r="BV3" s="11">
+        <v>5</v>
+      </c>
+      <c r="BW3" s="11">
+        <v>10</v>
+      </c>
+      <c r="BX3" s="11">
+        <v>10</v>
+      </c>
+      <c r="BY3" s="12">
         <v>30</v>
       </c>
-      <c r="BZ3" s="13">
-        <v>5</v>
-      </c>
-      <c r="CA3" s="13">
-        <v>10</v>
-      </c>
-      <c r="CB3" s="13">
+      <c r="BZ3" s="12">
+        <v>5</v>
+      </c>
+      <c r="CA3" s="12">
+        <v>10</v>
+      </c>
+      <c r="CB3" s="12">
         <v>20</v>
       </c>
-      <c r="CC3" s="13">
+      <c r="CC3" s="12">
         <v>20</v>
       </c>
-      <c r="CD3" s="12">
+      <c r="CD3" s="11">
         <v>30</v>
       </c>
-      <c r="CE3" s="12">
+      <c r="CE3" s="11">
         <v>30</v>
       </c>
-      <c r="CF3" s="12">
+      <c r="CF3" s="11">
         <v>20</v>
       </c>
-      <c r="CG3" s="12">
+      <c r="CG3" s="11">
         <v>20</v>
       </c>
-      <c r="CH3" s="12">
+      <c r="CH3" s="11">
         <v>35</v>
       </c>
-      <c r="CI3" s="12">
+      <c r="CI3" s="11">
         <v>40</v>
       </c>
-      <c r="CJ3" s="12">
+      <c r="CJ3" s="11">
         <f>SUM(F3,I3,AO3,AP3,AS3,AT3,AZ3:BC3,BY3:CI3)</f>
         <v>460</v>
       </c>
-      <c r="CK3" s="12">
+      <c r="CK3" s="11">
         <f>SUM(A3:CI3)</f>
         <v>1030</v>
       </c>
+    </row>
+    <row r="4" spans="1:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AF4" s="27"/>
+      <c r="AG4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AH4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AI4" s="27"/>
+      <c r="AJ4" s="27"/>
+      <c r="AK4" s="27"/>
+      <c r="AL4" s="27"/>
+      <c r="AM4" s="27"/>
+      <c r="AN4" s="27"/>
+      <c r="AO4" s="27"/>
+      <c r="AP4" s="27"/>
+      <c r="AQ4" s="27"/>
+      <c r="AR4" s="27"/>
+      <c r="AS4" s="27"/>
+      <c r="AT4" s="27"/>
+      <c r="AU4" s="27"/>
+      <c r="AV4" s="27"/>
+      <c r="AW4" s="27"/>
+      <c r="AX4" s="27"/>
+      <c r="AY4" s="27"/>
+      <c r="AZ4" s="27"/>
+      <c r="BA4" s="27"/>
+      <c r="BB4" s="27"/>
+      <c r="BC4" s="27"/>
+      <c r="BD4" s="27"/>
+      <c r="BE4" s="27"/>
+      <c r="BF4" s="27"/>
+      <c r="BG4" s="27"/>
+      <c r="BH4" s="27"/>
+      <c r="BI4" s="27"/>
+      <c r="BJ4" s="27"/>
+      <c r="BK4" s="27"/>
+      <c r="BL4" s="27"/>
+      <c r="BM4" s="27"/>
+      <c r="BN4" s="27"/>
+      <c r="BO4" s="27"/>
+      <c r="BP4" s="27"/>
+      <c r="BQ4" s="27"/>
+      <c r="BR4" s="27"/>
+      <c r="BS4" s="27"/>
+      <c r="BT4" s="27"/>
+      <c r="BU4" s="27"/>
+      <c r="BV4" s="27"/>
+      <c r="BW4" s="27"/>
+      <c r="BX4" s="27"/>
+      <c r="BY4" s="27"/>
+      <c r="BZ4" s="27"/>
+      <c r="CA4" s="27"/>
+      <c r="CB4" s="27"/>
+      <c r="CC4" s="27"/>
+      <c r="CD4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="CE4" s="27"/>
+      <c r="CF4" s="27"/>
+      <c r="CG4" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="CH4" s="27"/>
+      <c r="CI4" s="27"/>
+      <c r="CJ4" s="27"/>
+      <c r="CK4" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>